<commit_message>
add file to git ignore
</commit_message>
<xml_diff>
--- a/src/test/resources/DataExcel/ExcelData.xlsx
+++ b/src/test/resources/DataExcel/ExcelData.xlsx
@@ -5,14 +5,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId5"/>
+    <sheet name="Personal_Info" sheetId="1" r:id="rId4"/>
+    <sheet name="Product_Info" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29" count="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Email</t>
   </si>
@@ -79,34 +79,10 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>78</t>
+    <t>76</t>
   </si>
   <si>
     <t>77</t>
-  </si>
-  <si>
-    <t>76</t>
   </si>
 </sst>
 </file>
@@ -145,7 +121,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,9 +140,6 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill/>
-    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -339,7 +312,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -399,435 +372,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1889,9 +1433,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="25.3516"/>
-    <col min="2" max="9" customWidth="true" style="1" width="16.3516"/>
-    <col min="10" max="16384" customWidth="true" style="1" width="16.3516"/>
+    <col min="1" max="1" width="25.3516" style="1" customWidth="1"/>
+    <col min="2" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -2201,8 +1745,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" customWidth="true" style="13" width="16.3516"/>
-    <col min="6" max="16384" customWidth="true" style="13" width="16.3516"/>
+    <col min="1" max="5" width="16.3516" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.05" customHeight="1">
@@ -2223,33 +1767,33 @@
       </c>
     </row>
     <row r="2" ht="14.05" customHeight="1">
-      <c r="A2" t="s" s="155">
+      <c r="A2" t="s" s="14">
         <v>12</v>
       </c>
-      <c r="B2" t="s" s="156">
+      <c r="B2" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="C2" t="s" s="157">
+      <c r="C2" t="s" s="8">
         <v>14</v>
       </c>
-      <c r="D2" t="s" s="158">
+      <c r="D2" t="s" s="8">
         <v>15</v>
       </c>
-      <c r="E2" t="s" s="159">
-        <v>28</v>
+      <c r="E2" t="s" s="15">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="14.05" customHeight="1">
-      <c r="A3" t="s" s="160">
+      <c r="A3" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="161">
+      <c r="B3" t="s" s="12">
         <v>17</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" t="s" s="162">
-        <v>27</v>
+      <c r="E3" t="s" s="17">
+        <v>20</v>
       </c>
     </row>
     <row r="4" ht="14.05" customHeight="1">

</xml_diff>

<commit_message>
update element xpath and dependencies
</commit_message>
<xml_diff>
--- a/src/test/resources/DataExcel/ExcelData.xlsx
+++ b/src/test/resources/DataExcel/ExcelData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="13">
   <si>
     <t>Email</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>77</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +143,9 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill/>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -312,7 +318,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -372,6 +378,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1433,9 +1478,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.3516" style="1" customWidth="1"/>
-    <col min="2" max="9" width="16.3516" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="25.3516"/>
+    <col min="2" max="9" customWidth="true" style="1" width="16.3516"/>
+    <col min="10" max="16384" customWidth="true" style="1" width="16.3516"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1745,8 +1790,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="5" customWidth="true" style="13" width="16.3516"/>
+    <col min="6" max="16384" customWidth="true" style="13" width="16.3516"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.05" customHeight="1">
@@ -1767,33 +1812,33 @@
       </c>
     </row>
     <row r="2" ht="14.05" customHeight="1">
-      <c r="A2" t="s" s="14">
+      <c r="A2" t="s" s="25">
         <v>12</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" t="s" s="26">
         <v>13</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="C2" t="s" s="27">
         <v>14</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="D2" t="s" s="28">
         <v>15</v>
       </c>
-      <c r="E2" t="s" s="15">
+      <c r="E2" t="s" s="29">
         <v>19</v>
       </c>
     </row>
     <row r="3" ht="14.05" customHeight="1">
-      <c r="A3" t="s" s="16">
+      <c r="A3" t="s" s="30">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="12">
+      <c r="B3" t="s" s="31">
         <v>17</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" t="s" s="17">
-        <v>20</v>
+      <c r="E3" t="s" s="32">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="14.05" customHeight="1">

</xml_diff>